<commit_message>
More stuff for zika cds request ... adding resources for digital quality summit
</commit_message>
<xml_diff>
--- a/src/test/resources/org/opencds/cqf/zika-codesystem.xlsx
+++ b/src/test/resources/org/opencds/cqf/zika-codesystem.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="529">
   <si>
     <t>OID</t>
   </si>
@@ -908,18 +908,6 @@
     <t>Chikungunya virus Ab [Titer] in Serum by Hemagglutination inhibition</t>
   </si>
   <si>
-    <t>Chikungunya virus structural proteins (E1+E2) IgG Ab [Presence] in Serum 
-by Immunoassay</t>
-  </si>
-  <si>
-    <t>Chikungunya virus structural proteins (E1+E2) IgG Ab [Units/volume] in 
-Serum or Plasma by Immunoassay</t>
-  </si>
-  <si>
-    <t>Chikungunya virus structural proteins (E1+E2) IgM Ab [Units/volume] in 
-Serum or Plasma by Immunoassay</t>
-  </si>
-  <si>
     <t>Chikungunya virus IgG Ab [Presence] in Serum or Plasma by Immunofluorescence</t>
   </si>
   <si>
@@ -935,34 +923,6 @@
     <t>Chikungunya virus IgM Ab [Titer] in Serum or Plasma by Immunofluorescence</t>
   </si>
   <si>
-    <t>Chikungunya virus non-structural protein 1 (nsP1) RNA [Presence] in Cerebral 
-spinal fluid by Probe and target amplification method</t>
-  </si>
-  <si>
-    <t>Chikungunya virus non-structural protein 1 (nsP1) RNA [Presence] in Serum 
-by Probe and target amplification method</t>
-  </si>
-  <si>
-    <t>Chikungunya virus RNA [Presence] in Amniotic fluid by Probe and target 
-amplification method</t>
-  </si>
-  <si>
-    <t>Chikungunya virus RNA [Presence] in Serum or Plasma by Probe and target 
-amplification method</t>
-  </si>
-  <si>
-    <t>Chikungunya virus RNA [Presence] in Urine by Probe and target amplification 
-method</t>
-  </si>
-  <si>
-    <t>Chikungunya virus RNA [Presence] in Unspecified specimen by Probe and 
-target amplification method</t>
-  </si>
-  <si>
-    <t>Dengue and Chikungunya and Zika virus panel by Probe and target amplification 
-method</t>
-  </si>
-  <si>
     <t>34348001</t>
   </si>
   <si>
@@ -1627,6 +1587,33 @@
   </si>
   <si>
     <t>Zika virus RNA [Presence] in Unspecified specimen by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>Chikungunya virus structural proteins (E1+E2) IgG Ab [Presence] in Serum by Immunoassay</t>
+  </si>
+  <si>
+    <t>Chikungunya virus structural proteins (E1+E2) IgG Ab [Units/volume] in Serum or Plasma by Immunoassay</t>
+  </si>
+  <si>
+    <t>Chikungunya virus structural proteins (E1+E2) IgM Ab [Units/volume] in Serum or Plasma by Immunoassay</t>
+  </si>
+  <si>
+    <t>Chikungunya virus non-structural protein 1 (nsP1) RNA [Presence] in Serum by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>Chikungunya virus RNA [Presence] in Amniotic fluid by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>Chikungunya virus RNA [Presence] in Serum or Plasma by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>Chikungunya virus RNA [Presence] in Urine by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>Chikungunya virus RNA [Presence] in Unspecified specimen by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>Chikungunya virus non-structural protein 1 (nsP1) RNA [Presence] in Cerebral spinal fluid by Probe and target amplification method</t>
   </si>
 </sst>
 </file>
@@ -1975,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4233,7 +4220,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>209</v>
       </c>
@@ -4247,10 +4234,10 @@
         <v>274</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>209</v>
       </c>
@@ -4264,10 +4251,10 @@
         <v>275</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>209</v>
       </c>
@@ -4281,7 +4268,7 @@
         <v>276</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>295</v>
+        <v>522</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -4298,7 +4285,7 @@
         <v>277</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -4315,7 +4302,7 @@
         <v>278</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -4332,7 +4319,7 @@
         <v>279</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -4349,7 +4336,7 @@
         <v>280</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -4366,10 +4353,10 @@
         <v>281</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>209</v>
       </c>
@@ -4383,10 +4370,10 @@
         <v>282</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>209</v>
       </c>
@@ -4400,10 +4387,10 @@
         <v>283</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>209</v>
       </c>
@@ -4417,10 +4404,10 @@
         <v>284</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>209</v>
       </c>
@@ -4434,10 +4421,10 @@
         <v>285</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>209</v>
       </c>
@@ -4451,10 +4438,10 @@
         <v>286</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>209</v>
       </c>
@@ -4468,10 +4455,10 @@
         <v>287</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>209</v>
       </c>
@@ -4485,7 +4472,7 @@
         <v>288</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>307</v>
+        <v>430</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -4533,10 +4520,10 @@
         <v>129</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -4550,10 +4537,10 @@
         <v>129</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -4567,10 +4554,10 @@
         <v>129</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -4584,10 +4571,10 @@
         <v>129</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -4601,10 +4588,10 @@
         <v>129</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -4618,10 +4605,10 @@
         <v>129</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -4638,7 +4625,7 @@
         <v>288</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -4652,10 +4639,10 @@
         <v>211</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -4669,10 +4656,10 @@
         <v>211</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -4686,10 +4673,10 @@
         <v>211</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -4703,10 +4690,10 @@
         <v>211</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -4720,10 +4707,10 @@
         <v>211</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -4737,10 +4724,10 @@
         <v>211</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -4754,10 +4741,10 @@
         <v>211</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -4771,10 +4758,10 @@
         <v>211</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -4788,10 +4775,10 @@
         <v>211</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -4805,10 +4792,10 @@
         <v>211</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -4822,10 +4809,10 @@
         <v>211</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -4839,10 +4826,10 @@
         <v>211</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -4856,10 +4843,10 @@
         <v>211</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -4873,10 +4860,10 @@
         <v>211</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -4890,10 +4877,10 @@
         <v>211</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -4907,10 +4894,10 @@
         <v>211</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -4924,10 +4911,10 @@
         <v>211</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -4941,10 +4928,10 @@
         <v>211</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -4958,10 +4945,10 @@
         <v>211</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -4975,10 +4962,10 @@
         <v>211</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -4992,10 +4979,10 @@
         <v>211</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -5009,10 +4996,10 @@
         <v>211</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -5026,10 +5013,10 @@
         <v>211</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -5043,10 +5030,10 @@
         <v>211</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -5060,10 +5047,10 @@
         <v>211</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -5077,10 +5064,10 @@
         <v>211</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -5094,10 +5081,10 @@
         <v>211</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -5111,10 +5098,10 @@
         <v>211</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -5128,10 +5115,10 @@
         <v>211</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -5145,10 +5132,10 @@
         <v>211</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -5162,10 +5149,10 @@
         <v>211</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -5179,10 +5166,10 @@
         <v>211</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -5196,10 +5183,10 @@
         <v>211</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -5213,10 +5200,10 @@
         <v>211</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -5230,10 +5217,10 @@
         <v>211</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -5247,10 +5234,10 @@
         <v>211</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -5264,10 +5251,10 @@
         <v>211</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -5281,10 +5268,10 @@
         <v>211</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -5298,10 +5285,10 @@
         <v>211</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -5315,10 +5302,10 @@
         <v>211</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -5332,10 +5319,10 @@
         <v>211</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -5349,10 +5336,10 @@
         <v>211</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -5366,10 +5353,10 @@
         <v>211</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -5383,10 +5370,10 @@
         <v>211</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -5400,10 +5387,10 @@
         <v>211</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -5417,10 +5404,10 @@
         <v>211</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -5434,10 +5421,10 @@
         <v>211</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -5451,10 +5438,10 @@
         <v>211</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -5468,10 +5455,10 @@
         <v>211</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -5485,10 +5472,10 @@
         <v>211</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -5502,10 +5489,10 @@
         <v>211</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -5519,10 +5506,10 @@
         <v>211</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -5536,10 +5523,10 @@
         <v>211</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -5553,10 +5540,10 @@
         <v>211</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -5570,10 +5557,10 @@
         <v>211</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -5587,10 +5574,10 @@
         <v>211</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -5604,10 +5591,10 @@
         <v>211</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -5621,10 +5608,10 @@
         <v>211</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -5638,10 +5625,10 @@
         <v>211</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
@@ -5655,10 +5642,10 @@
         <v>211</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
@@ -5672,10 +5659,10 @@
         <v>211</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
@@ -5689,10 +5676,10 @@
         <v>211</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
@@ -5706,10 +5693,10 @@
         <v>211</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
@@ -5723,10 +5710,10 @@
         <v>211</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
@@ -5740,10 +5727,10 @@
         <v>211</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
@@ -5757,10 +5744,10 @@
         <v>211</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -5774,10 +5761,10 @@
         <v>211</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
@@ -5791,10 +5778,10 @@
         <v>211</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -5808,10 +5795,10 @@
         <v>211</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -5825,10 +5812,10 @@
         <v>211</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
@@ -5876,10 +5863,10 @@
         <v>129</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
@@ -5893,10 +5880,10 @@
         <v>129</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
@@ -5910,10 +5897,10 @@
         <v>129</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -5927,10 +5914,10 @@
         <v>129</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
@@ -5944,10 +5931,10 @@
         <v>130</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
@@ -5961,10 +5948,10 @@
         <v>129</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
@@ -5978,10 +5965,10 @@
         <v>129</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
@@ -5995,10 +5982,10 @@
         <v>129</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
@@ -6015,7 +6002,7 @@
         <v>84387000</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -6032,7 +6019,7 @@
         <v>271749004</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
@@ -6049,7 +6036,7 @@
         <v>47725002</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
@@ -6066,7 +6053,7 @@
         <v>57676002</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
@@ -6083,7 +6070,7 @@
         <v>9826008</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
@@ -6100,7 +6087,7 @@
         <v>68962001</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
@@ -6117,7 +6104,7 @@
         <v>25064002</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
@@ -6134,7 +6121,7 @@
         <v>288</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
@@ -6182,10 +6169,10 @@
         <v>211</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -6199,10 +6186,10 @@
         <v>211</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -6216,10 +6203,10 @@
         <v>211</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -6233,10 +6220,10 @@
         <v>211</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
@@ -6250,10 +6237,10 @@
         <v>211</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -6267,10 +6254,10 @@
         <v>211</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -6284,10 +6271,10 @@
         <v>211</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
@@ -6301,10 +6288,10 @@
         <v>211</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
@@ -6318,10 +6305,10 @@
         <v>211</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
@@ -6335,10 +6322,10 @@
         <v>211</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
@@ -6352,10 +6339,10 @@
         <v>211</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
@@ -6369,10 +6356,10 @@
         <v>211</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
@@ -6386,10 +6373,10 @@
         <v>211</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
@@ -6403,10 +6390,10 @@
         <v>211</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
@@ -6420,10 +6407,10 @@
         <v>211</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
@@ -6437,10 +6424,10 @@
         <v>211</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
@@ -6454,10 +6441,10 @@
         <v>211</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="E263" s="4" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
@@ -6471,10 +6458,10 @@
         <v>211</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
@@ -6488,10 +6475,10 @@
         <v>211</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
@@ -6505,10 +6492,10 @@
         <v>211</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
@@ -6522,10 +6509,10 @@
         <v>211</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
@@ -6539,10 +6526,10 @@
         <v>211</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
@@ -6556,10 +6543,10 @@
         <v>211</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
@@ -6573,10 +6560,10 @@
         <v>211</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
@@ -6590,10 +6577,10 @@
         <v>211</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
@@ -6607,10 +6594,10 @@
         <v>211</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>